<commit_message>
update default core #
</commit_message>
<xml_diff>
--- a/IO_M1_new/Reprod_RunControl_M1_new.xlsx
+++ b/IO_M1_new/Reprod_RunControl_M1_new.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7230" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7230" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="13" r:id="rId1"/>
@@ -1406,7 +1406,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1415,16 +1418,13 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2038,7 +2038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AY47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
@@ -2237,62 +2237,62 @@
       </c>
     </row>
     <row r="4" spans="1:51" s="8" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
       <c r="D4" s="42"/>
-      <c r="E4" s="50" t="s">
+      <c r="E4" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="50"/>
+      <c r="F4" s="46"/>
       <c r="G4" s="27"/>
       <c r="H4" s="27"/>
-      <c r="I4" s="51" t="s">
+      <c r="I4" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="46" t="s">
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="M4" s="46"/>
+      <c r="M4" s="47"/>
       <c r="N4" s="28"/>
-      <c r="O4" s="47" t="s">
+      <c r="O4" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="46" t="s">
+      <c r="P4" s="48"/>
+      <c r="Q4" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="R4" s="46"/>
-      <c r="S4" s="46"/>
-      <c r="T4" s="46"/>
-      <c r="U4" s="46"/>
-      <c r="V4" s="46"/>
-      <c r="W4" s="46"/>
-      <c r="X4" s="46"/>
+      <c r="R4" s="47"/>
+      <c r="S4" s="47"/>
+      <c r="T4" s="47"/>
+      <c r="U4" s="47"/>
+      <c r="V4" s="47"/>
+      <c r="W4" s="47"/>
+      <c r="X4" s="47"/>
       <c r="Y4" s="29"/>
       <c r="Z4" s="29"/>
-      <c r="AA4" s="47" t="s">
+      <c r="AA4" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="AB4" s="47"/>
-      <c r="AC4" s="47"/>
-      <c r="AD4" s="45" t="s">
+      <c r="AB4" s="48"/>
+      <c r="AC4" s="48"/>
+      <c r="AD4" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="AE4" s="45"/>
-      <c r="AF4" s="45"/>
+      <c r="AE4" s="50"/>
+      <c r="AF4" s="50"/>
       <c r="AG4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AH4" s="48" t="s">
+      <c r="AH4" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="AI4" s="48"/>
-      <c r="AJ4" s="48"/>
+      <c r="AI4" s="45"/>
+      <c r="AJ4" s="45"/>
       <c r="AK4" s="21" t="s">
         <v>70</v>
       </c>
@@ -2300,17 +2300,17 @@
       <c r="AM4" s="21"/>
       <c r="AN4" s="21"/>
       <c r="AO4" s="21"/>
-      <c r="AP4" s="45" t="s">
+      <c r="AP4" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="AQ4" s="45"/>
-      <c r="AR4" s="45"/>
-      <c r="AS4" s="49" t="s">
+      <c r="AQ4" s="50"/>
+      <c r="AR4" s="50"/>
+      <c r="AS4" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="AT4" s="49"/>
-      <c r="AU4" s="49"/>
-      <c r="AV4" s="49"/>
+      <c r="AT4" s="51"/>
+      <c r="AU4" s="51"/>
+      <c r="AV4" s="51"/>
       <c r="AW4" s="15"/>
       <c r="AX4" s="22"/>
       <c r="AY4" s="20"/>
@@ -7987,17 +7987,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="I4:K4"/>
     <mergeCell ref="AP4:AR4"/>
     <mergeCell ref="Q4:X4"/>
     <mergeCell ref="AA4:AC4"/>
     <mergeCell ref="AH4:AJ4"/>
     <mergeCell ref="AS4:AV4"/>
     <mergeCell ref="AD4:AF4"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="I4:K4"/>
   </mergeCells>
   <dataValidations count="21">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN6:AN47" xr:uid="{00000000-0002-0000-0200-000000000000}">
@@ -8356,8 +8356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>